<commit_message>
ça fonctionne bien maintenant. reste à vérifier que toutes les boîtes restent équilibrées, tester avec une forte demande d'énergie, ajouter des protections ou des options minimales si il n'y a pas de méthaniseurs.
</commit_message>
<xml_diff>
--- a/example/GRAFS_project_example_N.xlsx
+++ b/example/GRAFS_project_example_N.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8195474B-CFD1-4A69-83A2-D8450A6AEF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A881A15-0F0B-444B-AF59-E138D906E5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="4" xr2:uid="{092E5AC7-17CB-4282-9989-CDCB089F75B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{092E5AC7-17CB-4282-9989-CDCB089F75B9}"/>
   </bookViews>
   <sheets>
     <sheet name="crops" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
   <si>
     <t>Culture</t>
   </si>
@@ -1155,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CEBB00-B56F-4BED-97E3-E735E21789EF}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1169,9 +1169,10 @@
     <col min="4" max="4" width="12.453125" customWidth="1"/>
     <col min="6" max="6" width="12.7265625" customWidth="1"/>
     <col min="7" max="7" width="28.90625" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1193,8 +1194,11 @@
       <c r="G1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1210,8 +1214,11 @@
       <c r="G2">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1224,8 +1231,11 @@
       <c r="G3">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1238,8 +1248,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1252,8 +1265,11 @@
       <c r="G5">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1266,8 +1282,11 @@
       <c r="G6">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1278,6 +1297,9 @@
         <v>67</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -1290,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9008F097-1A19-4A13-A439-D292DC31E615}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1660,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986D1BE3-7A15-4223-93AE-9AB753B07534}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>